<commit_message>
Big update after report
</commit_message>
<xml_diff>
--- a/MLP_with_PSO/NN_output data/_fitness_results_uwoc_cosine.xlsx
+++ b/MLP_with_PSO/NN_output data/_fitness_results_uwoc_cosine.xlsx
@@ -441,252 +441,252 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.736407058323154</v>
+        <v>1.036527202731309</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.937334275667085</v>
+        <v>1.038842205395358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.314716415798638</v>
+        <v>1.326325506664252</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.247900499633087</v>
+        <v>1.779657095697206</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.517160752670951</v>
+        <v>1.809475044738209</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.615005110242942</v>
+        <v>1.663556186815498</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.895596126591656</v>
+        <v>1.702194396450396</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.942693353582118</v>
+        <v>1.947660774265794</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.945326314221286</v>
+        <v>1.983895126755568</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.849085735257499</v>
+        <v>1.850913905971616</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.702406207248427</v>
+        <v>1.590063071725434</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.497118744821764</v>
+        <v>1.336797387636375</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.390509920310689</v>
+        <v>1.194900433558507</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.355105472751214</v>
+        <v>1.059998552217474</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.229358960859947</v>
+        <v>0.9700298836639007</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.121985773286616</v>
+        <v>0.9068655966232724</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.064558626173392</v>
+        <v>0.8513422548435227</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.008314049387492</v>
+        <v>0.8252901890807021</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.9148990966404048</v>
+        <v>0.7929476054354004</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.8164424790714545</v>
+        <v>0.7749617135886168</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.7827440521906667</v>
+        <v>0.7596660551172044</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.7523327630738224</v>
+        <v>0.7341157469545613</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.7323062820679177</v>
+        <v>0.7181107202104252</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.7132886355813601</v>
+        <v>0.7103191777090804</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.7087730249842754</v>
+        <v>0.7038173918389828</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.7023464205250831</v>
+        <v>0.6989365637979807</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.6933369503368776</v>
+        <v>0.6932520569524969</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.6897147925129125</v>
+        <v>0.6910809928569983</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.6882349198936195</v>
+        <v>0.6875199864733751</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.6865886960204119</v>
+        <v>0.6861444759311689</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.6850515176143127</v>
+        <v>0.6842692588668601</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.6839865859250055</v>
+        <v>0.68330026243507</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.6827910299375705</v>
+        <v>0.6824158713357489</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.6823340432833371</v>
+        <v>0.6819083092044356</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.6820369495329222</v>
+        <v>0.6816123456854286</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.6818692496464613</v>
+        <v>0.6815023151766866</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.6815536485242318</v>
+        <v>0.6811745062053597</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.6814589758834477</v>
+        <v>0.6809586623367709</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.6813812595102745</v>
+        <v>0.6808763781609285</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.6813030939433993</v>
+        <v>0.6808466284810009</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.681248888500236</v>
+        <v>0.6807751233375516</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.6812368302083983</v>
+        <v>0.680758020328615</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.6811849961070797</v>
+        <v>0.6807259325172021</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.6811570785388658</v>
+        <v>0.6807052985319758</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.6811371460254116</v>
+        <v>0.6806873419142903</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.6811243427596205</v>
+        <v>0.6806737071097959</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.6811187877869145</v>
+        <v>0.6806676814022236</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.6811163671912802</v>
+        <v>0.6806608703856351</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.681109978157036</v>
+        <v>0.6806589824864423</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.6811087416756203</v>
+        <v>0.6806575008705177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>